<commit_message>
TP Módulo 1 - HTML:     [Entregado] Maquetación y estilos con tabla e imagenes
</commit_message>
<xml_diff>
--- a/modulo_1/src/Mediciones.xlsx
+++ b/modulo_1/src/Mediciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarav\Downloads\UTN\Professional_front_end_developer\modulo_1\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C8F1CF-144D-4D18-A533-5805EAA5B1E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBD9FAA-BB7B-4A69-836F-F075DC177B04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{85322208-1A2F-45A2-82CE-3C3A9C5D8E92}"/>
   </bookViews>
@@ -181,10 +181,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -230,13 +230,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -256,16 +262,30 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Potencia</c:v>
+            <c:strRef>
+              <c:f>Potencia!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Potencia [W]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -9279,7 +9299,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5DFE-41D3-AD7F-5D5F051EB26B}"/>
+              <c16:uniqueId val="{00000000-2F66-4F23-AC24-244ED05BC474}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9309,9 +9329,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -9325,9 +9345,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -9356,9 +9375,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -9384,9 +9403,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -9421,17 +9439,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -9468,6 +9497,37 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Temperatura [ºC]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9481,13 +9541,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -9518,13 +9584,19 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -14038,7 +14110,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D1AF-48C4-BCC8-2174541AFD62}"/>
+              <c16:uniqueId val="{00000000-2F66-4F23-AC24-244ED05BC474}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -14051,11 +14123,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="948563759"/>
-        <c:axId val="1029724431"/>
+        <c:axId val="946570431"/>
+        <c:axId val="933881951"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="948563759"/>
+        <c:axId val="946570431"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14068,9 +14140,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -14084,9 +14156,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -14097,7 +14168,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1029724431"/>
+        <c:crossAx val="933881951"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14105,7 +14176,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1029724431"/>
+        <c:axId val="933881951"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14115,9 +14186,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -14143,9 +14214,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -14156,7 +14226,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="948563759"/>
+        <c:crossAx val="946570431"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14170,27 +14240,32 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -14293,35 +14368,33 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -14329,26 +14402,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:chartArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -14357,9 +14438,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -14378,14 +14458,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -14394,45 +14466,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -14444,31 +14506,29 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -14486,21 +14546,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -14510,20 +14567,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -14537,14 +14594,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -14558,9 +14615,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -14574,12 +14630,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -14591,9 +14641,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -14608,14 +14658,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -14627,14 +14676,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -14646,14 +14695,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -14662,14 +14710,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -14677,7 +14724,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -14690,11 +14737,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -14702,14 +14759,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -14721,12 +14778,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -14742,7 +14806,6 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -14751,9 +14814,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -14763,7 +14825,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -14771,9 +14833,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -14784,9 +14846,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -14798,46 +14859,38 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -14845,26 +14898,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:chartArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -14873,9 +14934,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -14894,14 +14954,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -14910,45 +14962,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -14960,31 +15002,29 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -15002,21 +15042,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -15026,20 +15063,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -15053,14 +15090,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -15074,9 +15111,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -15090,12 +15126,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -15107,9 +15137,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -15124,14 +15154,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -15143,14 +15172,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -15162,14 +15191,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -15178,14 +15206,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -15193,7 +15220,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -15206,11 +15233,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -15218,14 +15255,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -15237,12 +15274,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -15258,7 +15302,6 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -15267,9 +15310,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -15279,7 +15321,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -15287,9 +15329,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -15300,9 +15342,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -15314,12 +15355,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -15329,26 +15364,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>589085</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A7D68AD-731A-4AE6-970D-E53D03BD5837}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{909DAF3D-033F-45B6-AA9B-A952A045F196}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -15375,10 +15412,10 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15706,7 +15743,7 @@
   <dimension ref="B4:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="B4:G25"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15715,90 +15752,90 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3">
+      <c r="C4" s="4"/>
+      <c r="D4" s="2">
         <v>30000</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
       <c r="E13" t="s">
         <v>17</v>
       </c>
@@ -15810,91 +15847,91 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
       <c r="G14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
       <c r="G15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
       <c r="G16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
       <c r="G17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
       <c r="G18" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
       <c r="G19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
       <c r="G20" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
       <c r="G21" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
       <c r="G22" t="s">
         <v>21</v>
       </c>
@@ -15909,6 +15946,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B22:D22"/>
@@ -15923,22 +15965,18 @@
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA82F0C-FC7F-4F50-BB4A-0D04BED5DF98}">
-  <dimension ref="A1:B3000"/>
+  <dimension ref="A1:L3000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D18" sqref="D4:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15947,7 +15985,7 @@
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15955,7 +15993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -15963,7 +16001,7 @@
         <v>1070.6399999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -15971,127 +16009,193 @@
         <v>1070.52</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4">
         <v>1073.52</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="K4">
+        <v>7</v>
+      </c>
+      <c r="L4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
         <v>1070.8799999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6">
         <v>1072.32</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7">
         <v>1072.08</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8">
         <v>1072.44</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9">
         <v>1071.96</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10">
         <v>1071</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11">
         <v>1071.1199999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12">
         <v>1068.48</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13">
         <v>1067.04</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14">
         <v>1067.3999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15">
         <v>1068</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16">
         <v>1070.52</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17">
         <v>1071.1199999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18">
         <v>1071.5999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -16099,7 +16203,7 @@
         <v>1070.8799999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -16107,7 +16211,7 @@
         <v>1072.08</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -16115,7 +16219,7 @@
         <v>1072.08</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -16123,7 +16227,7 @@
         <v>1071.8399999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -16131,7 +16235,7 @@
         <v>1070.6399999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -16139,7 +16243,7 @@
         <v>1071.48</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -16147,7 +16251,7 @@
         <v>1070.3999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -16155,7 +16259,7 @@
         <v>1068.48</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -16163,7 +16267,7 @@
         <v>1067.52</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -16171,7 +16275,7 @@
         <v>1067.6399999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -16179,7 +16283,7 @@
         <v>1066.92</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -16187,7 +16291,7 @@
         <v>1067.8799999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -16195,7 +16299,7 @@
         <v>1068.24</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -39956,10 +40060,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532F4E14-810F-49AA-8790-6A09C9A2DE0C}">
-  <dimension ref="A1:B3000"/>
+  <dimension ref="A1:L3000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39968,7 +40072,7 @@
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -39976,7 +40080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -39985,7 +40089,7 @@
         <v>30.400001664585414</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -39994,7 +40098,7 @@
         <v>30.79801330006655</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -40002,8 +40106,32 @@
         <f t="shared" si="0"/>
         <v>31.194044831754987</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="K4">
+        <v>7</v>
+      </c>
+      <c r="L4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -40011,8 +40139,11 @@
         <f t="shared" si="0"/>
         <v>31.588106135459579</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -40020,8 +40151,11 @@
         <f t="shared" si="0"/>
         <v>31.98020703773339</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -40029,8 +40163,11 @@
         <f t="shared" si="0"/>
         <v>32.370357316119346</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -40038,8 +40175,11 @@
         <f t="shared" si="0"/>
         <v>32.758566699394684</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -40047,8 +40187,11 @@
         <f t="shared" si="0"/>
         <v>33.14484486781415</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -40056,8 +40199,11 @@
         <f t="shared" si="0"/>
         <v>33.529201453352002</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -40065,8 +40211,11 @@
         <f t="shared" si="0"/>
         <v>33.911646039942873</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -40074,8 +40223,11 @@
         <f t="shared" si="0"/>
         <v>34.292188163721299</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -40083,8 +40235,11 @@
         <f t="shared" si="0"/>
         <v>34.670837313260101</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -40092,8 +40247,11 @@
         <f t="shared" si="0"/>
         <v>35.047602929807724</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -40101,8 +40259,11 @@
         <f t="shared" si="0"/>
         <v>35.422494407524141</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -40110,8 +40271,11 @@
         <f t="shared" si="0"/>
         <v>35.79552109371577</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -40119,8 +40283,11 @@
         <f t="shared" si="0"/>
         <v>36.16669228906914</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -40128,8 +40295,11 @@
         <f t="shared" si="0"/>
         <v>36.536017247883414</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -40138,7 +40308,7 @@
         <v>36.903505178301742</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -40147,7 +40317,7 @@
         <v>37.269165242541483</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -40156,7 +40326,7 @@
         <v>37.633006557123245</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -40165,7 +40335,7 @@
         <v>37.99503819309875</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -40174,7 +40344,7 @@
         <v>38.355269176277737</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -40183,7 +40353,7 @@
         <v>38.713708487453495</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -40192,7 +40362,7 @@
         <v>39.070365062627403</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -40201,7 +40371,7 @@
         <v>39.425247793232366</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -40210,7 +40380,7 @@
         <v>39.778365526355095</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -40219,7 +40389,7 @@
         <v>40.129727064957251</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -40228,7 +40398,7 @@
         <v>40.47934116809553</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -40237,7 +40407,7 @@
         <v>40.827216551140701</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -40246,7 +40416,7 @@
         <v>41.173361885995376</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -48630,7 +48800,7 @@
         <v>962</v>
       </c>
       <c r="B963">
-        <f t="shared" ref="B963:B1001" si="15">80*(1-EXP(-A963/200))+30+A963/1000</f>
+        <f t="shared" ref="B963:B1000" si="15">80*(1-EXP(-A963/200))+30+A963/1000</f>
         <v>110.31017122418561</v>
       </c>
     </row>
@@ -50133,7 +50303,7 @@
         <v>1129</v>
       </c>
       <c r="B1130">
-        <f t="shared" ref="B1130:B1193" si="18">(80*(EXP((-A1129+1500)/200))+30)/9.2</f>
+        <f t="shared" ref="B1130:B1139" si="18">(80*(EXP((-A1129+1500)/200))+30)/9.2</f>
         <v>59.119450186340309</v>
       </c>
     </row>

</xml_diff>